<commit_message>
feat: Add Employee issue
Added json files and csv files again and did changes in app_2.py for insert_employee
</commit_message>
<xml_diff>
--- a/backend/data/KPI/projects.xlsx
+++ b/backend/data/KPI/projects.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,225 +958,6 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>test kavindu</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Prediction Model</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Node.js</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>React</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>User Management</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>MERN</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>5</v>
-      </c>
-      <c r="M8" t="n">
-        <v>50000</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Wide</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>kavindu test complexcity</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>E-Commerce</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Recommendation Engine</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Node.js</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>React</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>User Management</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>MERN</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>5</v>
-      </c>
-      <c r="M9" t="n">
-        <v>50000</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">without complexcity </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>E-Commerce</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Prediction Model</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Node.js</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>React</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>User Management</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>MERN</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>7</v>
-      </c>
-      <c r="M10" t="n">
-        <v>70000</v>
-      </c>
-      <c r="N10" t="n">
-        <v>2</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>